<commit_message>
Found a document that have a little bit of practice
</commit_message>
<xml_diff>
--- a/data/Maths/Done.xlsx
+++ b/data/Maths/Done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyFiles\GitHub\S2024\Summer2024.github.io\data\Maths\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02962218-467D-47F5-94D9-518222F92788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E1F815-69B3-4712-BC2D-1A1ABA602B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1780,10 +1780,10 @@
       </c>
       <c r="G25" s="1">
         <f>H25/I25*100</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H25" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I25" s="2">
         <v>4</v>

</xml_diff>

<commit_message>
Added A latex folder for some stuff, and modified the correspondant excel files
</commit_message>
<xml_diff>
--- a/data/Maths/Done.xlsx
+++ b/data/Maths/Done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyFiles\GitHub\S2024\Summer2024.github.io\data\Maths\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E1F815-69B3-4712-BC2D-1A1ABA602B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8496BE48-88C9-421F-9B80-BFF735BE7E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -775,10 +775,10 @@
         <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>0</v>
@@ -837,13 +837,13 @@
       </c>
       <c r="L2" s="1">
         <f>M2/N2*100</f>
-        <v>0</v>
+        <v>1.5714285714285716</v>
       </c>
       <c r="M2" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N2" s="2">
-        <v>560</v>
+        <v>700</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>28</v>
@@ -878,10 +878,10 @@
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B10" si="0">C3/D3*100</f>
-        <v>10.670731707317072</v>
+        <v>12.5</v>
       </c>
       <c r="C3" s="2">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2">
         <v>328</v>
@@ -904,13 +904,13 @@
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L8" si="2">M3/N3*100</f>
-        <v>0</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="M3" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N3" s="2">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>29</v>
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="2">
-        <v>590</v>
+        <v>650</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>30</v>
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="2">
-        <v>485</v>
+        <v>450</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>31</v>
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="2">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>32</v>
@@ -1133,13 +1133,13 @@
       </c>
       <c r="L7" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="2">
-        <v>416</v>
+        <v>675</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>33</v>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="2">
-        <v>477</v>
+        <v>680</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="24" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>